<commit_message>
power plant data geupdate
</commit_message>
<xml_diff>
--- a/Power Plant Data.xlsx
+++ b/Power Plant Data.xlsx
@@ -5,69 +5,88 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piete\OneDrive\Documents\GitHub\EngineeringOptimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toon Stolk\Documents\Education\Space Engineering\Courses\ME46060 Engineering Optimization\Github Repository\EngineeringOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40659E0-70CB-45F1-91F2-929ACA0DB832}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B21708-0F27-45DE-9ED4-00AEFBC2D290}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Plant" sheetId="1" r:id="rId1"/>
-    <sheet name="Energy Requirements" sheetId="2" r:id="rId2"/>
+    <sheet name="Power Plant Normalized" sheetId="3" r:id="rId2"/>
+    <sheet name="Energy Requirements" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Power Plant</t>
   </si>
   <si>
-    <t>Coal</t>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>Hydro</t>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Solar</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
     <t>Biomass</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>tonnes CO2 per PJ</t>
-  </si>
-  <si>
-    <t>M euro Cost per PJ</t>
-  </si>
-  <si>
-    <t>Maintenance per PJ</t>
-  </si>
-  <si>
-    <t>Fuel cost per PJ</t>
-  </si>
-  <si>
-    <t>Oil</t>
+    <t>Coal w/o carbon capture</t>
+  </si>
+  <si>
+    <t>captial cost ($/kW)</t>
+  </si>
+  <si>
+    <t>Coal with 90% carbon capture</t>
+  </si>
+  <si>
+    <t>Combustion Turbines on gas</t>
+  </si>
+  <si>
+    <t>Combustion Turbines on gas with 90% carbon capture</t>
+  </si>
+  <si>
+    <t>Advanced Nuclear Power Plant</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>Hydroelectric power plant</t>
+  </si>
+  <si>
+    <t>Onshore Wind (small plant)</t>
+  </si>
+  <si>
+    <t>Offshore Wind</t>
+  </si>
+  <si>
+    <t>Solar Cell photovoltaic</t>
+  </si>
+  <si>
+    <t>Fixed O&amp;M Cost ($/kw-year)</t>
+  </si>
+  <si>
+    <t>Variable cost ($/MWh)</t>
+  </si>
+  <si>
+    <t>Variable cost ($/kWh)</t>
+  </si>
+  <si>
+    <t>C02(lb/MMBtu)</t>
+  </si>
+  <si>
+    <t>C02(kg/kWh)</t>
   </si>
 </sst>
 </file>
@@ -120,6 +139,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0CE4AED6-272C-4636-80AB-CCBD11143AA3}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0">
+  <autoFilter ref="A1:E12" xr:uid="{E830EB05-F720-4FC5-A29C-E776D937C1FE}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6998F321-CA2D-423C-937B-A621D7BFD7A8}" name="Power Plant"/>
+    <tableColumn id="2" xr3:uid="{0AA17703-3B8E-4EFA-BAF0-DFB5890E730F}" name="captial cost ($/kW)">
+      <calculatedColumnFormula>'Power Plant'!B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{F43DCDB8-DA91-4976-AC3E-81BED12FE935}" name="Fixed O&amp;M Cost ($/kw-year)">
+      <calculatedColumnFormula>'Power Plant'!C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{B72EAAED-F441-40C0-93EB-67B9D9AF0DC3}" name="Variable cost ($/kWh)">
+      <calculatedColumnFormula>'Power Plant'!D2*1000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C8525545-3234-48C8-BF40-B7D2FC025ED1}" name="C02(kg/kWh)">
+      <calculatedColumnFormula>'Power Plant'!E2*0.45359237/293.07107017222</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,79 +426,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>3676</v>
+      </c>
+      <c r="C2">
+        <v>40.58</v>
+      </c>
+      <c r="D2">
+        <v>4.5</v>
+      </c>
+      <c r="E2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5876</v>
+      </c>
+      <c r="C3">
+        <v>59.54</v>
+      </c>
+      <c r="D3">
+        <v>10.98</v>
+      </c>
+      <c r="E3">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1084</v>
+      </c>
+      <c r="C4">
+        <v>14.1</v>
+      </c>
+      <c r="D4">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2481</v>
+      </c>
+      <c r="C5">
+        <v>27.6</v>
+      </c>
+      <c r="D5">
+        <v>5.84</v>
+      </c>
+      <c r="E5">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>6041</v>
+      </c>
+      <c r="C6">
+        <v>121.64</v>
+      </c>
+      <c r="D6">
+        <v>2.37</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>4097</v>
+      </c>
+      <c r="C7">
+        <v>125.72</v>
+      </c>
+      <c r="D7">
+        <v>4.83</v>
+      </c>
+      <c r="E7">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>2521</v>
+      </c>
+      <c r="C8">
+        <v>128.54400000000001</v>
+      </c>
+      <c r="D8">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B9">
+        <v>5316</v>
+      </c>
+      <c r="C9">
+        <v>29.86</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B10">
+        <v>1677</v>
+      </c>
+      <c r="C10">
+        <v>35.14</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B11">
+        <v>4375</v>
+      </c>
+      <c r="C11">
+        <v>110</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
+      <c r="B12">
+        <v>1313</v>
+      </c>
+      <c r="C12">
+        <v>15.25</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -466,6 +651,279 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD7FDF1-0F3C-40D7-917F-CD8F60F46807}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <f>'Power Plant'!B2</f>
+        <v>3676</v>
+      </c>
+      <c r="C2">
+        <f>'Power Plant'!C2</f>
+        <v>40.58</v>
+      </c>
+      <c r="D2">
+        <f>'Power Plant'!D2*1000</f>
+        <v>4500</v>
+      </c>
+      <c r="E2">
+        <f>'Power Plant'!E2*0.45359237/293.07107017222</f>
+        <v>0.31883061049011419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f>'Power Plant'!B3</f>
+        <v>5876</v>
+      </c>
+      <c r="C3">
+        <f>'Power Plant'!C3</f>
+        <v>59.54</v>
+      </c>
+      <c r="D3">
+        <f>'Power Plant'!D3*1000</f>
+        <v>10980</v>
+      </c>
+      <c r="E3">
+        <f>'Power Plant'!E3*0.45359237/293.07107017222</f>
+        <v>3.1883061049011424E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>'Power Plant'!B4</f>
+        <v>1084</v>
+      </c>
+      <c r="C4">
+        <f>'Power Plant'!C4</f>
+        <v>14.1</v>
+      </c>
+      <c r="D4">
+        <f>'Power Plant'!D4*1000</f>
+        <v>2550</v>
+      </c>
+      <c r="E4">
+        <f>'Power Plant'!E4*0.45359237/293.07107017222</f>
+        <v>0.18108340498710371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <f>'Power Plant'!B5</f>
+        <v>2481</v>
+      </c>
+      <c r="C5">
+        <f>'Power Plant'!C5</f>
+        <v>27.6</v>
+      </c>
+      <c r="D5">
+        <f>'Power Plant'!D5*1000</f>
+        <v>5840</v>
+      </c>
+      <c r="E5">
+        <f>'Power Plant'!E5*0.45359237/293.07107017222</f>
+        <v>1.8108340498710369E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <f>'Power Plant'!B6</f>
+        <v>6041</v>
+      </c>
+      <c r="C6">
+        <f>'Power Plant'!C6</f>
+        <v>121.64</v>
+      </c>
+      <c r="D6">
+        <f>'Power Plant'!D6*1000</f>
+        <v>2370</v>
+      </c>
+      <c r="E6">
+        <f>'Power Plant'!E6*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <f>'Power Plant'!B7</f>
+        <v>4097</v>
+      </c>
+      <c r="C7">
+        <f>'Power Plant'!C7</f>
+        <v>125.72</v>
+      </c>
+      <c r="D7">
+        <f>'Power Plant'!D7*1000</f>
+        <v>4830</v>
+      </c>
+      <c r="E7">
+        <f>'Power Plant'!E7*0.45359237/293.07107017222</f>
+        <v>0.31883061049011419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f>'Power Plant'!B8</f>
+        <v>2521</v>
+      </c>
+      <c r="C8">
+        <f>'Power Plant'!C8</f>
+        <v>128.54400000000001</v>
+      </c>
+      <c r="D8">
+        <f>'Power Plant'!D8*1000</f>
+        <v>1160</v>
+      </c>
+      <c r="E8">
+        <f>'Power Plant'!E8*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <f>'Power Plant'!B9</f>
+        <v>5316</v>
+      </c>
+      <c r="C9">
+        <f>'Power Plant'!C9</f>
+        <v>29.86</v>
+      </c>
+      <c r="D9">
+        <f>'Power Plant'!D9*1000</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>'Power Plant'!E9*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f>'Power Plant'!B10</f>
+        <v>1677</v>
+      </c>
+      <c r="C10">
+        <f>'Power Plant'!C10</f>
+        <v>35.14</v>
+      </c>
+      <c r="D10">
+        <f>'Power Plant'!D10*1000</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>'Power Plant'!E10*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <f>'Power Plant'!B11</f>
+        <v>4375</v>
+      </c>
+      <c r="C11">
+        <f>'Power Plant'!C11</f>
+        <v>110</v>
+      </c>
+      <c r="D11">
+        <f>'Power Plant'!D11*1000</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>'Power Plant'!E11*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <f>'Power Plant'!B12</f>
+        <v>1313</v>
+      </c>
+      <c r="C12">
+        <f>'Power Plant'!C12</f>
+        <v>15.25</v>
+      </c>
+      <c r="D12">
+        <f>'Power Plant'!D12*1000</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>'Power Plant'!E12*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0434EE4-0B51-4A75-8BF2-2DBF37138733}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
added scenarios and first GA
</commit_message>
<xml_diff>
--- a/Power Plant Data.xlsx
+++ b/Power Plant Data.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toon Stolk\Documents\Education\Space Engineering\Courses\ME46060 Engineering Optimization\Github Repository\EngineeringOptimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piete\OneDrive\Documents\GitHub\EngineeringOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4B3124-2EEC-42CF-B3F8-F9EF468494D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D117F9-7235-42C6-9DAA-F3E0177C1E66}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Power Plant" sheetId="1" r:id="rId1"/>
-    <sheet name="Power Plant Normalized" sheetId="3" r:id="rId2"/>
+    <sheet name="Power Plant Normalized" sheetId="3" r:id="rId1"/>
+    <sheet name="Power Plant" sheetId="1" r:id="rId2"/>
     <sheet name="Production NL" sheetId="4" r:id="rId3"/>
     <sheet name="Energy Requirements" sheetId="2" r:id="rId4"/>
   </sheets>
@@ -484,11 +484,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD7FDF1-0F3C-40D7-917F-CD8F60F46807}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <f>'Power Plant'!B2</f>
+        <v>3676</v>
+      </c>
+      <c r="C2">
+        <f>'Power Plant'!C2</f>
+        <v>40.58</v>
+      </c>
+      <c r="D2">
+        <f>'Power Plant'!D2/1000</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="E2">
+        <f>'Power Plant'!E2*0.45359237/293.07107017222</f>
+        <v>0.31883061049011419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <f>'Power Plant'!B3</f>
+        <v>5876</v>
+      </c>
+      <c r="C3">
+        <f>'Power Plant'!C3</f>
+        <v>59.54</v>
+      </c>
+      <c r="D3">
+        <f>'Power Plant'!D3/1000</f>
+        <v>1.098E-2</v>
+      </c>
+      <c r="E3">
+        <f>'Power Plant'!E3*0.45359237/293.07107017222</f>
+        <v>3.1883061049011424E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <f>'Power Plant'!B4</f>
+        <v>1084</v>
+      </c>
+      <c r="C4">
+        <f>'Power Plant'!C4</f>
+        <v>14.1</v>
+      </c>
+      <c r="D4">
+        <f>'Power Plant'!D4/1000</f>
+        <v>2.5499999999999997E-3</v>
+      </c>
+      <c r="E4">
+        <f>'Power Plant'!E4*0.45359237/293.07107017222</f>
+        <v>0.18108340498710371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <f>'Power Plant'!B5</f>
+        <v>2481</v>
+      </c>
+      <c r="C5">
+        <f>'Power Plant'!C5</f>
+        <v>27.6</v>
+      </c>
+      <c r="D5">
+        <f>'Power Plant'!D5/1000</f>
+        <v>5.8399999999999997E-3</v>
+      </c>
+      <c r="E5">
+        <f>'Power Plant'!E5*0.45359237/293.07107017222</f>
+        <v>1.8108340498710369E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <f>'Power Plant'!B6</f>
+        <v>6041</v>
+      </c>
+      <c r="C6">
+        <f>'Power Plant'!C6</f>
+        <v>121.64</v>
+      </c>
+      <c r="D6">
+        <f>'Power Plant'!D6/1000</f>
+        <v>2.3700000000000001E-3</v>
+      </c>
+      <c r="E6">
+        <f>'Power Plant'!E6*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>'Power Plant'!B7</f>
+        <v>4097</v>
+      </c>
+      <c r="C7">
+        <f>'Power Plant'!C7</f>
+        <v>125.72</v>
+      </c>
+      <c r="D7">
+        <f>'Power Plant'!D7/1000</f>
+        <v>4.8300000000000001E-3</v>
+      </c>
+      <c r="E7">
+        <f>'Power Plant'!E7*0.45359237/293.07107017222</f>
+        <v>0.31883061049011419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <f>'Power Plant'!B8</f>
+        <v>2521</v>
+      </c>
+      <c r="C8">
+        <f>'Power Plant'!C8</f>
+        <v>128.54400000000001</v>
+      </c>
+      <c r="D8">
+        <f>'Power Plant'!D8/1000</f>
+        <v>1.16E-3</v>
+      </c>
+      <c r="E8">
+        <f>'Power Plant'!E8*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <f>'Power Plant'!B9</f>
+        <v>5316</v>
+      </c>
+      <c r="C9">
+        <f>'Power Plant'!C9</f>
+        <v>29.86</v>
+      </c>
+      <c r="D9">
+        <f>'Power Plant'!D9/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>'Power Plant'!E9*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <f>'Power Plant'!B10</f>
+        <v>1677</v>
+      </c>
+      <c r="C10">
+        <f>'Power Plant'!C10</f>
+        <v>35.14</v>
+      </c>
+      <c r="D10">
+        <f>'Power Plant'!D10/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>'Power Plant'!E10*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <f>'Power Plant'!B11</f>
+        <v>4375</v>
+      </c>
+      <c r="C11">
+        <f>'Power Plant'!C11</f>
+        <v>110</v>
+      </c>
+      <c r="D11">
+        <f>'Power Plant'!D11/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>'Power Plant'!E11*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <f>'Power Plant'!B12</f>
+        <v>1313</v>
+      </c>
+      <c r="C12">
+        <f>'Power Plant'!C12</f>
+        <v>15.25</v>
+      </c>
+      <c r="D12">
+        <f>'Power Plant'!D12/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>'Power Plant'!E12*0.45359237/293.07107017222</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,285 +982,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD7FDF1-0F3C-40D7-917F-CD8F60F46807}">
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <f>'Power Plant'!B2</f>
-        <v>3676</v>
-      </c>
-      <c r="C2">
-        <f>'Power Plant'!C2</f>
-        <v>40.58</v>
-      </c>
-      <c r="D2">
-        <f>'Power Plant'!D2/1000</f>
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="E2">
-        <f>'Power Plant'!E2*0.45359237/293.07107017222</f>
-        <v>0.31883061049011419</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <f>'Power Plant'!B3</f>
-        <v>5876</v>
-      </c>
-      <c r="C3">
-        <f>'Power Plant'!C3</f>
-        <v>59.54</v>
-      </c>
-      <c r="D3">
-        <f>'Power Plant'!D3/1000</f>
-        <v>1.098E-2</v>
-      </c>
-      <c r="E3">
-        <f>'Power Plant'!E3*0.45359237/293.07107017222</f>
-        <v>3.1883061049011424E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <f>'Power Plant'!B4</f>
-        <v>1084</v>
-      </c>
-      <c r="C4">
-        <f>'Power Plant'!C4</f>
-        <v>14.1</v>
-      </c>
-      <c r="D4">
-        <f>'Power Plant'!D4/1000</f>
-        <v>2.5499999999999997E-3</v>
-      </c>
-      <c r="E4">
-        <f>'Power Plant'!E4*0.45359237/293.07107017222</f>
-        <v>0.18108340498710371</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <f>'Power Plant'!B5</f>
-        <v>2481</v>
-      </c>
-      <c r="C5">
-        <f>'Power Plant'!C5</f>
-        <v>27.6</v>
-      </c>
-      <c r="D5">
-        <f>'Power Plant'!D5/1000</f>
-        <v>5.8399999999999997E-3</v>
-      </c>
-      <c r="E5">
-        <f>'Power Plant'!E5*0.45359237/293.07107017222</f>
-        <v>1.8108340498710369E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <f>'Power Plant'!B6</f>
-        <v>6041</v>
-      </c>
-      <c r="C6">
-        <f>'Power Plant'!C6</f>
-        <v>121.64</v>
-      </c>
-      <c r="D6">
-        <f>'Power Plant'!D6/1000</f>
-        <v>2.3700000000000001E-3</v>
-      </c>
-      <c r="E6">
-        <f>'Power Plant'!E6*0.45359237/293.07107017222</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <f>'Power Plant'!B7</f>
-        <v>4097</v>
-      </c>
-      <c r="C7">
-        <f>'Power Plant'!C7</f>
-        <v>125.72</v>
-      </c>
-      <c r="D7">
-        <f>'Power Plant'!D7/1000</f>
-        <v>4.8300000000000001E-3</v>
-      </c>
-      <c r="E7">
-        <f>'Power Plant'!E7*0.45359237/293.07107017222</f>
-        <v>0.31883061049011419</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <f>'Power Plant'!B8</f>
-        <v>2521</v>
-      </c>
-      <c r="C8">
-        <f>'Power Plant'!C8</f>
-        <v>128.54400000000001</v>
-      </c>
-      <c r="D8">
-        <f>'Power Plant'!D8/1000</f>
-        <v>1.16E-3</v>
-      </c>
-      <c r="E8">
-        <f>'Power Plant'!E8*0.45359237/293.07107017222</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <f>'Power Plant'!B9</f>
-        <v>5316</v>
-      </c>
-      <c r="C9">
-        <f>'Power Plant'!C9</f>
-        <v>29.86</v>
-      </c>
-      <c r="D9">
-        <f>'Power Plant'!D9/1000</f>
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f>'Power Plant'!E9*0.45359237/293.07107017222</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <f>'Power Plant'!B10</f>
-        <v>1677</v>
-      </c>
-      <c r="C10">
-        <f>'Power Plant'!C10</f>
-        <v>35.14</v>
-      </c>
-      <c r="D10">
-        <f>'Power Plant'!D10/1000</f>
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f>'Power Plant'!E10*0.45359237/293.07107017222</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <f>'Power Plant'!B11</f>
-        <v>4375</v>
-      </c>
-      <c r="C11">
-        <f>'Power Plant'!C11</f>
-        <v>110</v>
-      </c>
-      <c r="D11">
-        <f>'Power Plant'!D11/1000</f>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>'Power Plant'!E11*0.45359237/293.07107017222</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <f>'Power Plant'!B12</f>
-        <v>1313</v>
-      </c>
-      <c r="C12">
-        <f>'Power Plant'!C12</f>
-        <v>15.25</v>
-      </c>
-      <c r="D12">
-        <f>'Power Plant'!D12/1000</f>
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f>'Power Plant'!E12*0.45359237/293.07107017222</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5DFE38-936E-4457-AF38-EA84C8F96853}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,6 +1201,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>